<commit_message>
analysis of the solution
</commit_message>
<xml_diff>
--- a/GAP_results.xlsx
+++ b/GAP_results.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="gap results" sheetId="1" r:id="rId1"/>
+    <sheet name="method analysis" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Lower Bound</t>
   </si>
@@ -31,6 +32,15 @@
   </si>
   <si>
     <t>VRPTW</t>
+  </si>
+  <si>
+    <t>constructive</t>
+  </si>
+  <si>
+    <t>grasp alpha</t>
+  </si>
+  <si>
+    <t>grasp cardinality</t>
   </si>
 </sst>
 </file>
@@ -156,7 +166,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet!$A$2:$A$20</c:f>
+              <c:f>'gap results'!$A$2:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -222,7 +232,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet!$D$2:$D$20</c:f>
+              <c:f>'gap results'!$D$2:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -457,7 +467,620 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Amount</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of vehicles used</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'method analysis'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>constructive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'method analysis'!$B$2:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-25C2-474E-81CE-F34246D8661E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'method analysis'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>grasp alpha</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'method analysis'!$C$2:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-25C2-474E-81CE-F34246D8661E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'method analysis'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>grasp cardinality</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'method analysis'!$D$2:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-25C2-474E-81CE-F34246D8661E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="133970207"/>
+        <c:axId val="133972703"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="133970207"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="133972703"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="133972703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="133970207"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1013,6 +1636,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1027,6 +2166,41 @@
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1335,7 +2509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -1387,7 +2561,7 @@
         <v>138.99100000000001</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D29" si="0">(B3-C3)/B3*100</f>
+        <f t="shared" ref="D3:D20" si="0">(B3-C3)/B3*100</f>
         <v>62.458505859823411</v>
       </c>
     </row>
@@ -1650,4 +2824,300 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>13</v>
+      </c>
+      <c r="D16">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>37</v>
+      </c>
+      <c r="C17">
+        <v>34</v>
+      </c>
+      <c r="D17">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>27</v>
+      </c>
+      <c r="C19">
+        <v>29</v>
+      </c>
+      <c r="D19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>15</v>
+      </c>
+      <c r="C20">
+        <v>13</v>
+      </c>
+      <c r="D20">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>